<commit_message>
Modulus opdateret til Modulus Social. Vena har fået status godkendt for CPD-DK og XDS Metadata
</commit_message>
<xml_diff>
--- a/html/Apotekssystemer_excel.XLSX
+++ b/html/Apotekssystemer_excel.XLSX
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\GodkendteSystemer\html\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Godkendelsesdatabase\GodkendteSystemer\html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABBB026-1246-4079-ADEA-4A0F90F8BCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981EE06D-B1E6-46CA-9B3D-7210F7B992E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Opdateret d. 02-12-2025" sheetId="1" r:id="rId1"/>
+    <sheet name="Opdateret d. 05-12-2025" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Apotekssystemer">'Opdateret d. 02-12-2025'!$A$1:$E$9</definedName>
+    <definedName name="Apotekssystemer">'Opdateret d. 05-12-2025'!$A$1:$E$9</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -427,9 +427,9 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -463,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -480,7 +480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -494,7 +494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -511,7 +511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -528,7 +528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -545,7 +545,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -562,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>

</xml_diff>